<commit_message>
upload file and clean data code
</commit_message>
<xml_diff>
--- a/data/question_headers.xlsx
+++ b/data/question_headers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danie Smit\PycharmProjects\data-driven-org\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5E24FE-2652-49AA-B86A-02CAB886F546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F02BBC-1E1F-4292-99EB-AC3922009746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="322">
   <si>
     <t>Respondent ID</t>
   </si>
@@ -971,6 +971,21 @@
   </si>
   <si>
     <t>how_to_advant_visible</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>impo</t>
+  </si>
+  <si>
+    <t>agree</t>
+  </si>
+  <si>
+    <t>imp</t>
+  </si>
+  <si>
+    <t>Not at all important</t>
   </si>
 </sst>
 </file>
@@ -1379,8 +1394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DX125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DV1" workbookViewId="0">
-      <selection activeCell="DW12" sqref="DW12"/>
+    <sheetView tabSelected="1" topLeftCell="DP1" workbookViewId="0">
+      <selection activeCell="DP23" sqref="DP23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1481,14 +1496,7 @@
     <col min="118" max="118" width="148.85546875" bestFit="1" customWidth="1"/>
     <col min="119" max="119" width="90.5703125" bestFit="1" customWidth="1"/>
     <col min="120" max="120" width="61.85546875" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="224.85546875" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="229.85546875" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="183.28515625" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="104.7109375" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="101.85546875" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="117.7109375" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="246" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="85.7109375" bestFit="1" customWidth="1"/>
+    <col min="121" max="128" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:128" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -3444,15 +3452,102 @@
         <v>127</v>
       </c>
     </row>
+    <row r="8" spans="1:128" x14ac:dyDescent="0.25">
+      <c r="DQ8" t="s">
+        <v>317</v>
+      </c>
+      <c r="DR8" t="s">
+        <v>317</v>
+      </c>
+      <c r="DS8" t="s">
+        <v>317</v>
+      </c>
+      <c r="DT8" t="s">
+        <v>317</v>
+      </c>
+      <c r="DU8" t="s">
+        <v>317</v>
+      </c>
+      <c r="DV8" t="s">
+        <v>317</v>
+      </c>
+      <c r="DW8" t="s">
+        <v>317</v>
+      </c>
+      <c r="DX8" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:128" x14ac:dyDescent="0.25">
+      <c r="DQ10" t="s">
+        <v>318</v>
+      </c>
+      <c r="DR10" t="s">
+        <v>319</v>
+      </c>
+      <c r="DS10" t="s">
+        <v>318</v>
+      </c>
+      <c r="DT10" t="s">
+        <v>320</v>
+      </c>
+      <c r="DU10" t="s">
+        <v>319</v>
+      </c>
+      <c r="DV10" t="s">
+        <v>319</v>
+      </c>
+      <c r="DX10" t="s">
+        <v>319</v>
+      </c>
+    </row>
     <row r="11" spans="1:128" x14ac:dyDescent="0.25">
       <c r="CB11" t="s">
         <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:128" x14ac:dyDescent="0.25">
+      <c r="DQ12" t="s">
+        <v>171</v>
+      </c>
+      <c r="DR12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:128" x14ac:dyDescent="0.25">
+      <c r="DQ13" t="s">
+        <v>148</v>
+      </c>
+      <c r="DR13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:128" x14ac:dyDescent="0.25">
+      <c r="DQ14" t="s">
+        <v>147</v>
+      </c>
+      <c r="DR14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:128" x14ac:dyDescent="0.25">
+      <c r="DQ15" t="s">
+        <v>149</v>
+      </c>
+      <c r="DR15" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:128" x14ac:dyDescent="0.25">
       <c r="BL16" t="s">
         <v>204</v>
       </c>
+      <c r="DQ16" t="s">
+        <v>321</v>
+      </c>
+      <c r="DR16" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="20" spans="22:59" x14ac:dyDescent="0.25">
       <c r="BG20" t="s">
@@ -3476,5 +3571,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>